<commit_message>
Merging in Branch 1.5
git-svn-id: http://www.collectionstash.com/svn_collectionstash/trunk@613 3acffcf6-acfd-4bd8-953e-0dd6b9d92450
</commit_message>
<xml_diff>
--- a/doc/stickers.xlsx
+++ b/doc/stickers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Account Name</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>BuffyGirl</t>
+  </si>
+  <si>
+    <t>JC Kovacs
+12349 Metric Blvd #1330
+Austin, TX
+78758</t>
+  </si>
+  <si>
+    <t>King Darkness</t>
+  </si>
+  <si>
+    <t>Chase Valdez
+2418 East Highway 66
+PMB 539
+Gallup NM 87301</t>
   </si>
 </sst>
 </file>
@@ -436,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +539,9 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -530,6 +551,28 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>